<commit_message>
Terminada adaptação do rmap mem read e write
</commit_message>
<xml_diff>
--- a/FPGA_Developments/COM_Module_v1_5/References/NFEE_RMAP_Mem_VHDL_Big_Endian.xlsx
+++ b/FPGA_Developments/COM_Module_v1_5/References/NFEE_RMAP_Mem_VHDL_Big_Endian.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8DF78B-3485-4F08-9DA6-19940D00B630}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE797B9A-ACE5-4EA5-BAE0-B5A04CD81612}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register TREATED VHDL" sheetId="2" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t xml:space="preserve">  : </t>
   </si>
   <si>
-    <t>s_rmap_read_address</t>
-  </si>
-  <si>
     <t xml:space="preserve">signal </t>
   </si>
   <si>
@@ -186,9 +183,6 @@
   </si>
   <si>
     <t xml:space="preserve"> is</t>
-  </si>
-  <si>
-    <t>s_rmap_write_address</t>
   </si>
   <si>
     <t>rmap_config_registers_o</t>
@@ -418,6 +412,12 @@
   <si>
     <t>Default (VHDL)</t>
   </si>
+  <si>
+    <t>wr_addr_i(31 downto 0)</t>
+  </si>
+  <si>
+    <t>rd_addr_i(31 downto 0)</t>
+  </si>
 </sst>
 </file>
 
@@ -638,28 +638,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
@@ -3325,10 +3325,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>7</v>
@@ -3347,7 +3347,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="str">
+      <c r="B3" s="20" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]Registers TREATED'!C3,4),"""")</f>
         <v>x"00000000"</v>
       </c>
@@ -3385,7 +3385,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="17"/>
       <c r="D4" s="1" t="str">
         <f>'[1]Registers TREATED'!AG8</f>
@@ -3415,7 +3415,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="17"/>
       <c r="D5" s="1" t="str">
         <f>'[1]Registers TREATED'!AF8</f>
@@ -3445,7 +3445,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="17"/>
       <c r="D6" s="1" t="str">
         <f>'[1]Registers TREATED'!AE8</f>
@@ -3475,7 +3475,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="20"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="17"/>
       <c r="D7" s="16" t="str">
         <f>'[1]Registers TREATED'!O8</f>
@@ -3506,7 +3506,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17" t="str">
@@ -3533,7 +3533,7 @@
       <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="20"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18" t="str">
@@ -3560,7 +3560,7 @@
       <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="20"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="17"/>
       <c r="D10" s="16" t="str">
         <f>'[1]Registers TREATED'!C8</f>
@@ -3777,11 +3777,11 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="str">
+      <c r="B17" s="20" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]Registers TREATED'!C19,4),"""")</f>
         <v>x"00000008"</v>
       </c>
-      <c r="C17" s="19" t="str">
+      <c r="C17" s="20" t="str">
         <f>'[1]Registers TREATED'!C18:AH18</f>
         <v>spw_packet_1_config</v>
       </c>
@@ -3815,8 +3815,8 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="1" t="str">
         <f>'[1]Registers TREATED'!AG24</f>
         <v>digitise_control</v>
@@ -3848,8 +3848,8 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="1" t="str">
         <f>'[1]Registers TREATED'!AE24</f>
         <v>ccd_port_data_transmission_selection_control</v>
@@ -3882,8 +3882,8 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="16" t="str">
         <f>'[1]Registers TREATED'!O24</f>
         <v>packet_size_control</v>
@@ -3916,8 +3916,8 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17" t="str">
         <f>IF('[1]Register TREATED TABLE'!E21="-","-",IF(MID('[1]Register TREATED TABLE'!E21,2,1)="x",CONCATENATE("x""",RIGHT('[1]Register TREATED TABLE'!E21,LEN('[1]Register TREATED TABLE'!E21)-2),""""),IF(MID('[1]Register TREATED TABLE'!E21,2,1)="b",CONCATENATE("""",RIGHT('[1]Register TREATED TABLE'!E21,LEN('[1]Register TREATED TABLE'!E21)-2),""""),IF(H21="-",CONCATENATE("'",'[1]Register TREATED TABLE'!E21,"'"),CONCATENATE("(others =&gt; '",'[1]Register TREATED TABLE'!E21,"')")))))</f>
@@ -3943,8 +3943,8 @@
       <c r="K21" s="17"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="18"/>
       <c r="E22" s="18" t="str">
         <f>IF('[1]Register TREATED TABLE'!E22="-","-",IF(MID('[1]Register TREATED TABLE'!E22,2,1)="x",CONCATENATE("x""",RIGHT('[1]Register TREATED TABLE'!E22,LEN('[1]Register TREATED TABLE'!E22)-2),""""),IF(MID('[1]Register TREATED TABLE'!E22,2,1)="b",CONCATENATE("""",RIGHT('[1]Register TREATED TABLE'!E22,LEN('[1]Register TREATED TABLE'!E22)-2),""""),IF(H22="-",CONCATENATE("'",'[1]Register TREATED TABLE'!E22,"'"),CONCATENATE("(others =&gt; '",'[1]Register TREATED TABLE'!E22,"')")))))</f>
@@ -3970,8 +3970,8 @@
       <c r="K22" s="18"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="16" t="s">
         <v>1</v>
       </c>
@@ -4003,8 +4003,8 @@
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18" t="str">
         <f>IF('[1]Register TREATED TABLE'!E24="-","-",IF(MID('[1]Register TREATED TABLE'!E24,2,1)="x",CONCATENATE("x""",RIGHT('[1]Register TREATED TABLE'!E24,LEN('[1]Register TREATED TABLE'!E24)-2),""""),IF(MID('[1]Register TREATED TABLE'!E24,2,1)="b",CONCATENATE("""",RIGHT('[1]Register TREATED TABLE'!E24,LEN('[1]Register TREATED TABLE'!E24)-2),""""),IF(H24="-",CONCATENATE("'",'[1]Register TREATED TABLE'!E24,"'"),CONCATENATE("(others =&gt; '",'[1]Register TREATED TABLE'!E24,"')")))))</f>
@@ -6046,7 +6046,7 @@
       <c r="D89" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E89" s="21" t="str">
+      <c r="E89" s="19" t="str">
         <f>IF('[1]Register TREATED TABLE'!E89="-","-",IF(MID('[1]Register TREATED TABLE'!E89,2,1)="x",CONCATENATE("x""",RIGHT('[1]Register TREATED TABLE'!E89,LEN('[1]Register TREATED TABLE'!E89)-2),""""),IF(MID('[1]Register TREATED TABLE'!E89,2,1)="b",CONCATENATE("""",RIGHT('[1]Register TREATED TABLE'!E89,LEN('[1]Register TREATED TABLE'!E89)-2),""""),IF(H89="-",CONCATENATE("'",'[1]Register TREATED TABLE'!E89,"'"),CONCATENATE("(others =&gt; '",'[1]Register TREATED TABLE'!E89,"')")))))</f>
         <v>(others =&gt; '0')</v>
       </c>
@@ -6310,6 +6310,133 @@
     </row>
   </sheetData>
   <mergeCells count="151">
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="C49:C52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="B43:B48"/>
+    <mergeCell ref="C74:C79"/>
+    <mergeCell ref="B74:B79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="C69:C73"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="F17:F20"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="F74:F76"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="B17:B24"/>
+    <mergeCell ref="C17:C24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="C93:C97"/>
+    <mergeCell ref="B93:B97"/>
+    <mergeCell ref="D94:D97"/>
+    <mergeCell ref="E94:E97"/>
+    <mergeCell ref="C88:C92"/>
+    <mergeCell ref="B88:B92"/>
+    <mergeCell ref="D89:D92"/>
+    <mergeCell ref="E89:E92"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C63:C68"/>
+    <mergeCell ref="B63:B68"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="B53:B58"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C3:C11"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="F94:F95"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="J89:J92"/>
+    <mergeCell ref="J25:J28"/>
+    <mergeCell ref="J29:J32"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="J39:J42"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="J49:J52"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="K84:K87"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="J59:J62"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="J71:J73"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="J84:J87"/>
     <mergeCell ref="K89:K92"/>
     <mergeCell ref="K94:K97"/>
     <mergeCell ref="K49:K52"/>
@@ -6334,133 +6461,6 @@
     <mergeCell ref="K47:K48"/>
     <mergeCell ref="K71:K73"/>
     <mergeCell ref="K76:K79"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="K84:K87"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="J59:J62"/>
-    <mergeCell ref="J64:J65"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="J71:J73"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="J84:J87"/>
-    <mergeCell ref="J89:J92"/>
-    <mergeCell ref="J25:J28"/>
-    <mergeCell ref="J29:J32"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="J39:J42"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="J49:J52"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="F94:F95"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C3:C11"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C93:C97"/>
-    <mergeCell ref="B93:B97"/>
-    <mergeCell ref="D94:D97"/>
-    <mergeCell ref="E94:E97"/>
-    <mergeCell ref="C88:C92"/>
-    <mergeCell ref="B88:B92"/>
-    <mergeCell ref="D89:D92"/>
-    <mergeCell ref="E89:E92"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C63:C68"/>
-    <mergeCell ref="B63:B68"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C53:C58"/>
-    <mergeCell ref="B53:B58"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="F17:F20"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="F74:F76"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="B17:B24"/>
-    <mergeCell ref="C17:C24"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C43:C48"/>
-    <mergeCell ref="B43:B48"/>
-    <mergeCell ref="C74:C79"/>
-    <mergeCell ref="B74:B79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="C69:C73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8957,7 +8957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U179"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8981,18 +8981,18 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -9012,7 +9012,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U2" t="str">
         <f>CONCATENATE(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2)</f>
@@ -9021,13 +9021,13 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -9058,7 +9058,7 @@
         <v>17</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U3" t="str">
         <f>CONCATENATE(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3,P3,Q3,R3,S3)</f>
@@ -9067,15 +9067,15 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>38</v>
@@ -9113,7 +9113,7 @@
       </c>
       <c r="U6" t="str">
         <f>CONCATENATE(B6,C6,D6,E6,F6,G6,H6,I6,J6,K6,L6,M6,N6,O6,P6,Q6,R6,S6)</f>
-        <v>signal s_rmap_read_address  : std_logic_vector(31 downto 0);</v>
+        <v>signal rd_addr_i(31 downto 0)  : std_logic_vector(31 downto 0);</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -9127,7 +9127,7 @@
       </c>
       <c r="C9" s="7" t="str">
         <f>C6</f>
-        <v>s_rmap_read_address</v>
+        <v>rd_addr_i(31 downto 0)</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>34</v>
@@ -9149,7 +9149,7 @@
       <c r="S9" s="5"/>
       <c r="U9" t="str">
         <f t="shared" ref="U9:U40" si="0">CONCATENATE(B9,C9,D9,E9,F9,G9,H9,I9,J9,K9,L9,M9,N9,O9,P9,Q9,R9,S9)</f>
-        <v>case (s_rmap_read_address) is</v>
+        <v>case (rd_addr_i(31 downto 0)) is</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -12771,12 +12771,8 @@
       <c r="K83" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L83" s="9">
-        <v>0</v>
-      </c>
-      <c r="M83" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
       <c r="N83" s="5"/>
       <c r="O83" s="5"/>
       <c r="P83" s="5"/>
@@ -12787,7 +12783,7 @@
       </c>
       <c r="U83" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">    rmap_readdata_o(7 downto 4) &lt;= ( others =&gt; '0')0');</v>
+        <v xml:space="preserve">    rmap_readdata_o(7 downto 4) &lt;= ( others =&gt; '0');</v>
       </c>
     </row>
     <row r="84" spans="2:21" x14ac:dyDescent="0.3">
@@ -17168,7 +17164,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X199"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X199" sqref="X170:X199"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -17198,18 +17196,18 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -17243,7 +17241,7 @@
         <v>17</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X2" t="str">
         <f>CONCATENATE(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2)</f>
@@ -17252,13 +17250,13 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -17281,7 +17279,7 @@
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X3" t="str">
         <f>CONCATENATE(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3,P3,Q3,R3,S3,T3,U3,V3)</f>
@@ -17290,15 +17288,15 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>38</v>
@@ -17339,7 +17337,7 @@
       </c>
       <c r="X6" t="str">
         <f>CONCATENATE(B6,C6,D6,E6,F6,G6,H6,I6,J6,K6,L6,M6,N6,O6,P6,Q6,R6,S6,T6,U6,V6)</f>
-        <v>signal s_rmap_write_address  : std_logic_vector(31 downto 0);</v>
+        <v>signal wr_addr_i(31 downto 0)  : std_logic_vector(31 downto 0);</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
@@ -17353,13 +17351,13 @@
       </c>
       <c r="C9" s="7" t="str">
         <f>$C$6</f>
-        <v>s_rmap_write_address</v>
+        <v>wr_addr_i(31 downto 0)</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -17380,7 +17378,7 @@
       <c r="V9" s="5"/>
       <c r="X9" t="str">
         <f t="shared" ref="X9:X40" si="0">CONCATENATE(B9,C9,D9,E9,F9,G9,H9,I9,J9,K9,L9,M9,N9,O9,P9,Q9,R9,S9,T9,U9,V9)</f>
-        <v>case (s_rmap_write_address) is</v>
+        <v>case (wr_addr_i(31 downto 0)) is</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -18416,7 +18414,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -18921,7 +18919,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -18994,7 +18992,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -19067,7 +19065,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -19140,7 +19138,7 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -19213,7 +19211,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -23006,7 +23004,7 @@
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
       <c r="G119" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H119" s="5"/>
       <c r="I119" s="5"/>
@@ -23079,7 +23077,7 @@
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
       <c r="G121" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H121" s="5"/>
       <c r="I121" s="5"/>
@@ -23152,7 +23150,7 @@
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
       <c r="G123" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H123" s="5"/>
       <c r="I123" s="5"/>
@@ -23379,7 +23377,7 @@
       <c r="E128" s="5"/>
       <c r="F128" s="5"/>
       <c r="G128" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
@@ -23452,7 +23450,7 @@
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
       <c r="G130" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H130" s="5"/>
       <c r="I130" s="5"/>
@@ -23525,7 +23523,7 @@
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
       <c r="G132" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H132" s="5"/>
       <c r="I132" s="5"/>
@@ -23598,7 +23596,7 @@
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
       <c r="G134" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H134" s="5"/>
       <c r="I134" s="5"/>
@@ -23671,7 +23669,7 @@
       <c r="E136" s="5"/>
       <c r="F136" s="5"/>
       <c r="G136" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H136" s="5"/>
       <c r="I136" s="5"/>
@@ -23744,7 +23742,7 @@
       <c r="E138" s="5"/>
       <c r="F138" s="5"/>
       <c r="G138" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H138" s="5"/>
       <c r="I138" s="5"/>
@@ -23817,7 +23815,7 @@
       <c r="E140" s="5"/>
       <c r="F140" s="5"/>
       <c r="G140" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H140" s="5"/>
       <c r="I140" s="5"/>
@@ -23890,7 +23888,7 @@
       <c r="E142" s="5"/>
       <c r="F142" s="5"/>
       <c r="G142" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H142" s="5"/>
       <c r="I142" s="5"/>
@@ -23963,7 +23961,7 @@
       <c r="E144" s="5"/>
       <c r="F144" s="5"/>
       <c r="G144" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
@@ -24036,7 +24034,7 @@
       <c r="E146" s="5"/>
       <c r="F146" s="5"/>
       <c r="G146" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H146" s="5"/>
       <c r="I146" s="5"/>
@@ -24109,7 +24107,7 @@
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
       <c r="G148" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H148" s="5"/>
       <c r="I148" s="5"/>
@@ -24278,7 +24276,7 @@
       <c r="E152" s="5"/>
       <c r="F152" s="5"/>
       <c r="G152" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H152" s="5"/>
       <c r="I152" s="5"/>
@@ -24351,7 +24349,7 @@
       <c r="E154" s="5"/>
       <c r="F154" s="5"/>
       <c r="G154" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H154" s="5"/>
       <c r="I154" s="5"/>
@@ -24424,7 +24422,7 @@
       <c r="E156" s="5"/>
       <c r="F156" s="5"/>
       <c r="G156" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H156" s="5"/>
       <c r="I156" s="5"/>
@@ -24593,7 +24591,7 @@
       <c r="E160" s="5"/>
       <c r="F160" s="5"/>
       <c r="G160" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H160" s="5"/>
       <c r="I160" s="5"/>
@@ -24666,7 +24664,7 @@
       <c r="E162" s="5"/>
       <c r="F162" s="5"/>
       <c r="G162" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H162" s="5"/>
       <c r="I162" s="5"/>
@@ -24739,7 +24737,7 @@
       <c r="E164" s="5"/>
       <c r="F164" s="5"/>
       <c r="G164" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H164" s="5"/>
       <c r="I164" s="5"/>
@@ -24809,7 +24807,7 @@
       <c r="E166" s="5"/>
       <c r="F166" s="5"/>
       <c r="G166" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H166" s="5"/>
       <c r="I166" s="5"/>
@@ -24864,7 +24862,7 @@
     </row>
     <row r="169" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A169" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="170" spans="1:24" x14ac:dyDescent="0.3">
@@ -25278,7 +25276,9 @@
         <f>'Register TREATED VHDL'!C17</f>
         <v>spw_packet_1_config</v>
       </c>
-      <c r="J178" s="8"/>
+      <c r="J178" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="K178" s="9" t="str">
         <f>'Register TREATED VHDL'!D20</f>
         <v>packet_size_control</v>
@@ -25303,7 +25303,7 @@
       </c>
       <c r="X178" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">  rmap_config_registers_o.spw_packet_1_configpacket_size_control &lt;= x"11F8";</v>
+        <v xml:space="preserve">  rmap_config_registers_o.spw_packet_1_config.packet_size_control &lt;= x"11F8";</v>
       </c>
     </row>
     <row r="179" spans="2:24" x14ac:dyDescent="0.3">
@@ -26344,7 +26344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -26362,20 +26362,20 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="25" t="str">
+      <c r="B3" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="23" t="str">
         <f>IF('[1]HK TREATED'!E3="-","-",IF(MID('[1]HK TREATED'!E3,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E3,LEN('[1]HK TREATED'!E3)-2),""""),IF(MID('[1]HK TREATED'!E3,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E3,LEN('[1]HK TREATED'!E3)-2),""""),IF(H3="-",CONCATENATE("'",'[1]HK TREATED'!E3,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E3,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26385,18 +26385,18 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F4,4),"""")</f>
         <v>x"00000702"</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="25" t="str">
+      <c r="B5" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="23" t="str">
         <f>IF('[1]HK TREATED'!E5="-","-",IF(MID('[1]HK TREATED'!E5,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E5,LEN('[1]HK TREATED'!E5)-2),""""),IF(MID('[1]HK TREATED'!E5,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E5,LEN('[1]HK TREATED'!E5)-2),""""),IF(H5="-",CONCATENATE("'",'[1]HK TREATED'!E5,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E5,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26406,20 +26406,20 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="26"/>
+      <c r="B6" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="24"/>
       <c r="D6" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F6,4),"""")</f>
         <v>x"00000700"</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="25" t="str">
+      <c r="B7" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="23" t="str">
         <f>IF('[1]HK TREATED'!E7="-","-",IF(MID('[1]HK TREATED'!E7,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E7,LEN('[1]HK TREATED'!E7)-2),""""),IF(MID('[1]HK TREATED'!E7,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E7,LEN('[1]HK TREATED'!E7)-2),""""),IF(H7="-",CONCATENATE("'",'[1]HK TREATED'!E7,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E7,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26429,20 +26429,20 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="26"/>
+      <c r="B8" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="24"/>
       <c r="D8" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F8,4),"""")</f>
         <v>x"00000706"</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="25" t="str">
+      <c r="B9" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="23" t="str">
         <f>IF('[1]HK TREATED'!E9="-","-",IF(MID('[1]HK TREATED'!E9,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E9,LEN('[1]HK TREATED'!E9)-2),""""),IF(MID('[1]HK TREATED'!E9,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E9,LEN('[1]HK TREATED'!E9)-2),""""),IF(H9="-",CONCATENATE("'",'[1]HK TREATED'!E9,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E9,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26452,20 +26452,20 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="26"/>
+      <c r="B10" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="24"/>
       <c r="D10" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F10,4),"""")</f>
         <v>x"00000704"</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="C11" s="25" t="str">
+      <c r="B11" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="23" t="str">
         <f>IF('[1]HK TREATED'!E11="-","-",IF(MID('[1]HK TREATED'!E11,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E11,LEN('[1]HK TREATED'!E11)-2),""""),IF(MID('[1]HK TREATED'!E11,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E11,LEN('[1]HK TREATED'!E11)-2),""""),IF(H11="-",CONCATENATE("'",'[1]HK TREATED'!E11,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E11,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26475,20 +26475,20 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="26"/>
+      <c r="B12" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="24"/>
       <c r="D12" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F12,4),"""")</f>
         <v>x"0000070A"</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" s="25" t="str">
+      <c r="B13" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="23" t="str">
         <f>IF('[1]HK TREATED'!E13="-","-",IF(MID('[1]HK TREATED'!E13,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E13,LEN('[1]HK TREATED'!E13)-2),""""),IF(MID('[1]HK TREATED'!E13,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E13,LEN('[1]HK TREATED'!E13)-2),""""),IF(H13="-",CONCATENATE("'",'[1]HK TREATED'!E13,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E13,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26498,20 +26498,20 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="26"/>
+      <c r="B14" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="24"/>
       <c r="D14" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F14,4),"""")</f>
         <v>x"00000708"</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="25" t="str">
+      <c r="B15" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="23" t="str">
         <f>IF('[1]HK TREATED'!E15="-","-",IF(MID('[1]HK TREATED'!E15,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E15,LEN('[1]HK TREATED'!E15)-2),""""),IF(MID('[1]HK TREATED'!E15,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E15,LEN('[1]HK TREATED'!E15)-2),""""),IF(H15="-",CONCATENATE("'",'[1]HK TREATED'!E15,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E15,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26521,20 +26521,20 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="26"/>
+      <c r="B16" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="24"/>
       <c r="D16" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F16,4),"""")</f>
         <v>x"0000070E"</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="25" t="str">
+      <c r="B17" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="23" t="str">
         <f>IF('[1]HK TREATED'!E17="-","-",IF(MID('[1]HK TREATED'!E17,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E17,LEN('[1]HK TREATED'!E17)-2),""""),IF(MID('[1]HK TREATED'!E17,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E17,LEN('[1]HK TREATED'!E17)-2),""""),IF(H17="-",CONCATENATE("'",'[1]HK TREATED'!E17,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E17,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26544,20 +26544,20 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" s="26"/>
+      <c r="B18" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="24"/>
       <c r="D18" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F18,4),"""")</f>
         <v>x"0000070C"</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" s="25" t="str">
+      <c r="B19" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="23" t="str">
         <f>IF('[1]HK TREATED'!E19="-","-",IF(MID('[1]HK TREATED'!E19,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E19,LEN('[1]HK TREATED'!E19)-2),""""),IF(MID('[1]HK TREATED'!E19,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E19,LEN('[1]HK TREATED'!E19)-2),""""),IF(H19="-",CONCATENATE("'",'[1]HK TREATED'!E19,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E19,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26567,20 +26567,20 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="26"/>
+      <c r="B20" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="24"/>
       <c r="D20" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F20,4),"""")</f>
         <v>x"00000712"</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="25" t="str">
+      <c r="B21" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="23" t="str">
         <f>IF('[1]HK TREATED'!E21="-","-",IF(MID('[1]HK TREATED'!E21,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E21,LEN('[1]HK TREATED'!E21)-2),""""),IF(MID('[1]HK TREATED'!E21,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E21,LEN('[1]HK TREATED'!E21)-2),""""),IF(H21="-",CONCATENATE("'",'[1]HK TREATED'!E21,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E21,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26590,20 +26590,20 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" s="26"/>
+      <c r="B22" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="24"/>
       <c r="D22" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F22,4),"""")</f>
         <v>x"00000710"</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="25" t="str">
+      <c r="B23" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="23" t="str">
         <f>IF('[1]HK TREATED'!E23="-","-",IF(MID('[1]HK TREATED'!E23,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E23,LEN('[1]HK TREATED'!E23)-2),""""),IF(MID('[1]HK TREATED'!E23,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E23,LEN('[1]HK TREATED'!E23)-2),""""),IF(H23="-",CONCATENATE("'",'[1]HK TREATED'!E23,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E23,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26613,20 +26613,20 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="26"/>
+      <c r="B24" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="24"/>
       <c r="D24" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F24,4),"""")</f>
         <v>x"00000716"</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" s="25" t="str">
+      <c r="B25" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="23" t="str">
         <f>IF('[1]HK TREATED'!E25="-","-",IF(MID('[1]HK TREATED'!E25,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E25,LEN('[1]HK TREATED'!E25)-2),""""),IF(MID('[1]HK TREATED'!E25,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E25,LEN('[1]HK TREATED'!E25)-2),""""),IF(H25="-",CONCATENATE("'",'[1]HK TREATED'!E25,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E25,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26636,20 +26636,20 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="26"/>
+      <c r="B26" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="24"/>
       <c r="D26" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F26,4),"""")</f>
         <v>x"00000714"</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="25" t="str">
+      <c r="B27" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="23" t="str">
         <f>IF('[1]HK TREATED'!E27="-","-",IF(MID('[1]HK TREATED'!E27,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E27,LEN('[1]HK TREATED'!E27)-2),""""),IF(MID('[1]HK TREATED'!E27,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E27,LEN('[1]HK TREATED'!E27)-2),""""),IF(H27="-",CONCATENATE("'",'[1]HK TREATED'!E27,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E27,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26659,20 +26659,20 @@
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="26"/>
+      <c r="B28" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="24"/>
       <c r="D28" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F28,4),"""")</f>
         <v>x"0000071A"</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="25" t="str">
+      <c r="B29" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="23" t="str">
         <f>IF('[1]HK TREATED'!E29="-","-",IF(MID('[1]HK TREATED'!E29,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E29,LEN('[1]HK TREATED'!E29)-2),""""),IF(MID('[1]HK TREATED'!E29,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E29,LEN('[1]HK TREATED'!E29)-2),""""),IF(H29="-",CONCATENATE("'",'[1]HK TREATED'!E29,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E29,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26682,20 +26682,20 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" s="26"/>
+      <c r="B30" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="24"/>
       <c r="D30" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F30,4),"""")</f>
         <v>x"00000718"</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" s="25" t="str">
+      <c r="B31" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="23" t="str">
         <f>IF('[1]HK TREATED'!E31="-","-",IF(MID('[1]HK TREATED'!E31,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E31,LEN('[1]HK TREATED'!E31)-2),""""),IF(MID('[1]HK TREATED'!E31,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E31,LEN('[1]HK TREATED'!E31)-2),""""),IF(H31="-",CONCATENATE("'",'[1]HK TREATED'!E31,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E31,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26705,20 +26705,20 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C32" s="26"/>
+      <c r="B32" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="24"/>
       <c r="D32" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F32,4),"""")</f>
         <v>x"0000071E"</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="25" t="str">
+      <c r="B33" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="23" t="str">
         <f>IF('[1]HK TREATED'!E33="-","-",IF(MID('[1]HK TREATED'!E33,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E33,LEN('[1]HK TREATED'!E33)-2),""""),IF(MID('[1]HK TREATED'!E33,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E33,LEN('[1]HK TREATED'!E33)-2),""""),IF(H33="-",CONCATENATE("'",'[1]HK TREATED'!E33,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E33,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26728,20 +26728,20 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="26"/>
+      <c r="B34" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="24"/>
       <c r="D34" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F34,4),"""")</f>
         <v>x"0000071C"</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="25" t="str">
+      <c r="B35" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="23" t="str">
         <f>IF('[1]HK TREATED'!E35="-","-",IF(MID('[1]HK TREATED'!E35,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E35,LEN('[1]HK TREATED'!E35)-2),""""),IF(MID('[1]HK TREATED'!E35,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E35,LEN('[1]HK TREATED'!E35)-2),""""),IF(H35="-",CONCATENATE("'",'[1]HK TREATED'!E35,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E35,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26751,20 +26751,20 @@
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C36" s="26"/>
+      <c r="B36" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="24"/>
       <c r="D36" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F36,4),"""")</f>
         <v>x"00000722"</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="25" t="str">
+      <c r="B37" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="23" t="str">
         <f>IF('[1]HK TREATED'!E37="-","-",IF(MID('[1]HK TREATED'!E37,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E37,LEN('[1]HK TREATED'!E37)-2),""""),IF(MID('[1]HK TREATED'!E37,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E37,LEN('[1]HK TREATED'!E37)-2),""""),IF(H37="-",CONCATENATE("'",'[1]HK TREATED'!E37,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E37,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26774,20 +26774,20 @@
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="26"/>
+      <c r="B38" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="24"/>
       <c r="D38" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F38,4),"""")</f>
         <v>x"00000720"</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="25" t="str">
+      <c r="B39" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="23" t="str">
         <f>IF('[1]HK TREATED'!E39="-","-",IF(MID('[1]HK TREATED'!E39,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E39,LEN('[1]HK TREATED'!E39)-2),""""),IF(MID('[1]HK TREATED'!E39,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E39,LEN('[1]HK TREATED'!E39)-2),""""),IF(H39="-",CONCATENATE("'",'[1]HK TREATED'!E39,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E39,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26797,20 +26797,20 @@
       </c>
     </row>
     <row r="40" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" s="26"/>
+      <c r="B40" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="24"/>
       <c r="D40" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F40,4),"""")</f>
         <v>x"00000726"</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="25" t="str">
+      <c r="B41" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="23" t="str">
         <f>IF('[1]HK TREATED'!E41="-","-",IF(MID('[1]HK TREATED'!E41,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E41,LEN('[1]HK TREATED'!E41)-2),""""),IF(MID('[1]HK TREATED'!E41,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E41,LEN('[1]HK TREATED'!E41)-2),""""),IF(H41="-",CONCATENATE("'",'[1]HK TREATED'!E41,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E41,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26820,20 +26820,20 @@
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="26"/>
+      <c r="B42" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="24"/>
       <c r="D42" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F42,4),"""")</f>
         <v>x"00000724"</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="25" t="str">
+      <c r="B43" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="23" t="str">
         <f>IF('[1]HK TREATED'!E43="-","-",IF(MID('[1]HK TREATED'!E43,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E43,LEN('[1]HK TREATED'!E43)-2),""""),IF(MID('[1]HK TREATED'!E43,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E43,LEN('[1]HK TREATED'!E43)-2),""""),IF(H43="-",CONCATENATE("'",'[1]HK TREATED'!E43,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E43,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26843,20 +26843,20 @@
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" s="26"/>
+      <c r="B44" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="24"/>
       <c r="D44" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F44,4),"""")</f>
         <v>x"0000072A"</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="25" t="str">
+      <c r="B45" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="23" t="str">
         <f>IF('[1]HK TREATED'!E45="-","-",IF(MID('[1]HK TREATED'!E45,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E45,LEN('[1]HK TREATED'!E45)-2),""""),IF(MID('[1]HK TREATED'!E45,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E45,LEN('[1]HK TREATED'!E45)-2),""""),IF(H45="-",CONCATENATE("'",'[1]HK TREATED'!E45,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E45,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26866,20 +26866,20 @@
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="26"/>
+      <c r="B46" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="24"/>
       <c r="D46" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F46,4),"""")</f>
         <v>x"00000728"</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C47" s="25" t="str">
+      <c r="B47" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="23" t="str">
         <f>IF('[1]HK TREATED'!E47="-","-",IF(MID('[1]HK TREATED'!E47,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E47,LEN('[1]HK TREATED'!E47)-2),""""),IF(MID('[1]HK TREATED'!E47,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E47,LEN('[1]HK TREATED'!E47)-2),""""),IF(H47="-",CONCATENATE("'",'[1]HK TREATED'!E47,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E47,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26889,20 +26889,20 @@
       </c>
     </row>
     <row r="48" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" s="26"/>
+      <c r="B48" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="24"/>
       <c r="D48" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F48,4),"""")</f>
         <v>x"0000072E"</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="25" t="str">
+      <c r="B49" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="23" t="str">
         <f>IF('[1]HK TREATED'!E49="-","-",IF(MID('[1]HK TREATED'!E49,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E49,LEN('[1]HK TREATED'!E49)-2),""""),IF(MID('[1]HK TREATED'!E49,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E49,LEN('[1]HK TREATED'!E49)-2),""""),IF(H49="-",CONCATENATE("'",'[1]HK TREATED'!E49,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E49,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26912,20 +26912,20 @@
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="26"/>
+      <c r="B50" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="24"/>
       <c r="D50" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F50,4),"""")</f>
         <v>x"0000072C"</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="25" t="str">
+      <c r="B51" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="23" t="str">
         <f>IF('[1]HK TREATED'!E51="-","-",IF(MID('[1]HK TREATED'!E51,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E51,LEN('[1]HK TREATED'!E51)-2),""""),IF(MID('[1]HK TREATED'!E51,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E51,LEN('[1]HK TREATED'!E51)-2),""""),IF(H51="-",CONCATENATE("'",'[1]HK TREATED'!E51,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E51,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26935,20 +26935,20 @@
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="26"/>
+      <c r="B52" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="24"/>
       <c r="D52" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F52,4),"""")</f>
         <v>x"00000732"</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B53" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" s="25" t="str">
+      <c r="B53" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="23" t="str">
         <f>IF('[1]HK TREATED'!E53="-","-",IF(MID('[1]HK TREATED'!E53,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E53,LEN('[1]HK TREATED'!E53)-2),""""),IF(MID('[1]HK TREATED'!E53,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E53,LEN('[1]HK TREATED'!E53)-2),""""),IF(H53="-",CONCATENATE("'",'[1]HK TREATED'!E53,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E53,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26958,20 +26958,20 @@
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54" s="26"/>
+      <c r="B54" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="24"/>
       <c r="D54" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F54,4),"""")</f>
         <v>x"00000730"</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="25" t="str">
+      <c r="B55" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="23" t="str">
         <f>IF('[1]HK TREATED'!E55="-","-",IF(MID('[1]HK TREATED'!E55,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E55,LEN('[1]HK TREATED'!E55)-2),""""),IF(MID('[1]HK TREATED'!E55,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E55,LEN('[1]HK TREATED'!E55)-2),""""),IF(H55="-",CONCATENATE("'",'[1]HK TREATED'!E55,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E55,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -26981,20 +26981,20 @@
       </c>
     </row>
     <row r="56" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="26"/>
+      <c r="B56" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="24"/>
       <c r="D56" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F56,4),"""")</f>
         <v>x"00000736"</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C57" s="25" t="str">
+      <c r="B57" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="23" t="str">
         <f>IF('[1]HK TREATED'!E57="-","-",IF(MID('[1]HK TREATED'!E57,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E57,LEN('[1]HK TREATED'!E57)-2),""""),IF(MID('[1]HK TREATED'!E57,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E57,LEN('[1]HK TREATED'!E57)-2),""""),IF(H57="-",CONCATENATE("'",'[1]HK TREATED'!E57,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E57,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27004,20 +27004,20 @@
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C58" s="26"/>
+      <c r="B58" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="24"/>
       <c r="D58" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F58,4),"""")</f>
         <v>x"00000734"</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B59" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="25" t="str">
+      <c r="B59" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" s="23" t="str">
         <f>IF('[1]HK TREATED'!E59="-","-",IF(MID('[1]HK TREATED'!E59,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E59,LEN('[1]HK TREATED'!E59)-2),""""),IF(MID('[1]HK TREATED'!E59,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E59,LEN('[1]HK TREATED'!E59)-2),""""),IF(H59="-",CONCATENATE("'",'[1]HK TREATED'!E59,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E59,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27027,20 +27027,20 @@
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C60" s="26"/>
+      <c r="B60" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="24"/>
       <c r="D60" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F60,4),"""")</f>
         <v>x"0000073A"</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B61" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" s="25" t="str">
+      <c r="B61" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="23" t="str">
         <f>IF('[1]HK TREATED'!E61="-","-",IF(MID('[1]HK TREATED'!E61,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E61,LEN('[1]HK TREATED'!E61)-2),""""),IF(MID('[1]HK TREATED'!E61,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E61,LEN('[1]HK TREATED'!E61)-2),""""),IF(H61="-",CONCATENATE("'",'[1]HK TREATED'!E61,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E61,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27050,20 +27050,20 @@
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B62" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C62" s="26"/>
+      <c r="B62" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" s="24"/>
       <c r="D62" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F62,4),"""")</f>
         <v>x"00000738"</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B63" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" s="25" t="str">
+      <c r="B63" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="23" t="str">
         <f>IF('[1]HK TREATED'!E63="-","-",IF(MID('[1]HK TREATED'!E63,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E63,LEN('[1]HK TREATED'!E63)-2),""""),IF(MID('[1]HK TREATED'!E63,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E63,LEN('[1]HK TREATED'!E63)-2),""""),IF(H63="-",CONCATENATE("'",'[1]HK TREATED'!E63,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E63,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27073,20 +27073,20 @@
       </c>
     </row>
     <row r="64" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C64" s="26"/>
+      <c r="B64" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64" s="24"/>
       <c r="D64" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F64,4),"""")</f>
         <v>x"0000073E"</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B65" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C65" s="25" t="str">
+      <c r="B65" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="23" t="str">
         <f>IF('[1]HK TREATED'!E65="-","-",IF(MID('[1]HK TREATED'!E65,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E65,LEN('[1]HK TREATED'!E65)-2),""""),IF(MID('[1]HK TREATED'!E65,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E65,LEN('[1]HK TREATED'!E65)-2),""""),IF(H65="-",CONCATENATE("'",'[1]HK TREATED'!E65,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E65,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27096,20 +27096,20 @@
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B66" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C66" s="26"/>
+      <c r="B66" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="24"/>
       <c r="D66" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F66,4),"""")</f>
         <v>x"0000073C"</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B67" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C67" s="25" t="str">
+      <c r="B67" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C67" s="23" t="str">
         <f>IF('[1]HK TREATED'!E67="-","-",IF(MID('[1]HK TREATED'!E67,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E67,LEN('[1]HK TREATED'!E67)-2),""""),IF(MID('[1]HK TREATED'!E67,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E67,LEN('[1]HK TREATED'!E67)-2),""""),IF(H67="-",CONCATENATE("'",'[1]HK TREATED'!E67,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E67,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27119,20 +27119,20 @@
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B68" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C68" s="26"/>
+      <c r="B68" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" s="24"/>
       <c r="D68" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F68,4),"""")</f>
         <v>x"00000742"</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B69" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C69" s="25" t="str">
+      <c r="B69" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="23" t="str">
         <f>IF('[1]HK TREATED'!E69="-","-",IF(MID('[1]HK TREATED'!E69,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E69,LEN('[1]HK TREATED'!E69)-2),""""),IF(MID('[1]HK TREATED'!E69,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E69,LEN('[1]HK TREATED'!E69)-2),""""),IF(H69="-",CONCATENATE("'",'[1]HK TREATED'!E69,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E69,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27142,20 +27142,20 @@
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B70" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C70" s="26"/>
+      <c r="B70" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" s="24"/>
       <c r="D70" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F70,4),"""")</f>
         <v>x"00000740"</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B71" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C71" s="25" t="str">
+      <c r="B71" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="23" t="str">
         <f>IF('[1]HK TREATED'!E71="-","-",IF(MID('[1]HK TREATED'!E71,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E71,LEN('[1]HK TREATED'!E71)-2),""""),IF(MID('[1]HK TREATED'!E71,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E71,LEN('[1]HK TREATED'!E71)-2),""""),IF(H71="-",CONCATENATE("'",'[1]HK TREATED'!E71,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E71,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27165,20 +27165,20 @@
       </c>
     </row>
     <row r="72" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" s="26"/>
+      <c r="B72" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="24"/>
       <c r="D72" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F72,4),"""")</f>
         <v>x"00000746"</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B73" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C73" s="25" t="str">
+      <c r="B73" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73" s="23" t="str">
         <f>IF('[1]HK TREATED'!E73="-","-",IF(MID('[1]HK TREATED'!E73,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E73,LEN('[1]HK TREATED'!E73)-2),""""),IF(MID('[1]HK TREATED'!E73,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E73,LEN('[1]HK TREATED'!E73)-2),""""),IF(H73="-",CONCATENATE("'",'[1]HK TREATED'!E73,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E73,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27188,20 +27188,20 @@
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B74" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" s="26"/>
+      <c r="B74" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74" s="24"/>
       <c r="D74" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F74,4),"""")</f>
         <v>x"00000744"</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B75" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C75" s="25" t="str">
+      <c r="B75" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" s="23" t="str">
         <f>IF('[1]HK TREATED'!E75="-","-",IF(MID('[1]HK TREATED'!E75,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E75,LEN('[1]HK TREATED'!E75)-2),""""),IF(MID('[1]HK TREATED'!E75,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E75,LEN('[1]HK TREATED'!E75)-2),""""),IF(H75="-",CONCATENATE("'",'[1]HK TREATED'!E75,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E75,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27211,20 +27211,20 @@
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B76" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C76" s="26"/>
+      <c r="B76" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76" s="24"/>
       <c r="D76" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F76,4),"""")</f>
         <v>x"0000074A"</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B77" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C77" s="25" t="str">
+      <c r="B77" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" s="23" t="str">
         <f>IF('[1]HK TREATED'!E77="-","-",IF(MID('[1]HK TREATED'!E77,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E77,LEN('[1]HK TREATED'!E77)-2),""""),IF(MID('[1]HK TREATED'!E77,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E77,LEN('[1]HK TREATED'!E77)-2),""""),IF(H77="-",CONCATENATE("'",'[1]HK TREATED'!E77,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E77,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27234,20 +27234,20 @@
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B78" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C78" s="26"/>
+      <c r="B78" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78" s="24"/>
       <c r="D78" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F78,4),"""")</f>
         <v>x"00000748"</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B79" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C79" s="25" t="str">
+      <c r="B79" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" s="23" t="str">
         <f>IF('[1]HK TREATED'!E79="-","-",IF(MID('[1]HK TREATED'!E79,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E79,LEN('[1]HK TREATED'!E79)-2),""""),IF(MID('[1]HK TREATED'!E79,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E79,LEN('[1]HK TREATED'!E79)-2),""""),IF(H79="-",CONCATENATE("'",'[1]HK TREATED'!E79,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E79,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27257,20 +27257,20 @@
       </c>
     </row>
     <row r="80" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C80" s="26"/>
+      <c r="B80" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" s="24"/>
       <c r="D80" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F80,4),"""")</f>
         <v>x"0000074E"</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B81" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="C81" s="25" t="str">
+      <c r="B81" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C81" s="23" t="str">
         <f>IF('[1]HK TREATED'!E81="-","-",IF(MID('[1]HK TREATED'!E81,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E81,LEN('[1]HK TREATED'!E81)-2),""""),IF(MID('[1]HK TREATED'!E81,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E81,LEN('[1]HK TREATED'!E81)-2),""""),IF(H81="-",CONCATENATE("'",'[1]HK TREATED'!E81,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E81,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27280,20 +27280,20 @@
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B82" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="C82" s="26"/>
+      <c r="B82" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C82" s="24"/>
       <c r="D82" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F82,4),"""")</f>
         <v>x"0000074C"</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B83" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C83" s="25" t="str">
+      <c r="B83" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C83" s="23" t="str">
         <f>IF('[1]HK TREATED'!E83="-","-",IF(MID('[1]HK TREATED'!E83,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E83,LEN('[1]HK TREATED'!E83)-2),""""),IF(MID('[1]HK TREATED'!E83,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E83,LEN('[1]HK TREATED'!E83)-2),""""),IF(H83="-",CONCATENATE("'",'[1]HK TREATED'!E83,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E83,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27303,20 +27303,20 @@
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B84" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C84" s="26"/>
+      <c r="B84" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C84" s="24"/>
       <c r="D84" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F84,4),"""")</f>
         <v>x"00000752"</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B85" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C85" s="25" t="str">
+      <c r="B85" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C85" s="23" t="str">
         <f>IF('[1]HK TREATED'!E85="-","-",IF(MID('[1]HK TREATED'!E85,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E85,LEN('[1]HK TREATED'!E85)-2),""""),IF(MID('[1]HK TREATED'!E85,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E85,LEN('[1]HK TREATED'!E85)-2),""""),IF(H85="-",CONCATENATE("'",'[1]HK TREATED'!E85,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E85,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27326,20 +27326,20 @@
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B86" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C86" s="26"/>
+      <c r="B86" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C86" s="24"/>
       <c r="D86" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F86,4),"""")</f>
         <v>x"00000750"</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B87" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C87" s="25" t="str">
+      <c r="B87" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C87" s="23" t="str">
         <f>IF('[1]HK TREATED'!E87="-","-",IF(MID('[1]HK TREATED'!E87,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E87,LEN('[1]HK TREATED'!E87)-2),""""),IF(MID('[1]HK TREATED'!E87,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E87,LEN('[1]HK TREATED'!E87)-2),""""),IF(H87="-",CONCATENATE("'",'[1]HK TREATED'!E87,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E87,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27349,20 +27349,20 @@
       </c>
     </row>
     <row r="88" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C88" s="26"/>
+      <c r="B88" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C88" s="24"/>
       <c r="D88" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F88,4),"""")</f>
         <v>x"00000756"</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B89" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C89" s="25" t="str">
+      <c r="B89" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" s="23" t="str">
         <f>IF('[1]HK TREATED'!E89="-","-",IF(MID('[1]HK TREATED'!E89,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E89,LEN('[1]HK TREATED'!E89)-2),""""),IF(MID('[1]HK TREATED'!E89,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E89,LEN('[1]HK TREATED'!E89)-2),""""),IF(H89="-",CONCATENATE("'",'[1]HK TREATED'!E89,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E89,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27372,20 +27372,20 @@
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B90" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C90" s="26"/>
+      <c r="B90" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C90" s="24"/>
       <c r="D90" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F90,4),"""")</f>
         <v>x"00000754"</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B91" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C91" s="25" t="str">
+      <c r="B91" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C91" s="23" t="str">
         <f>IF('[1]HK TREATED'!E91="-","-",IF(MID('[1]HK TREATED'!E91,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E91,LEN('[1]HK TREATED'!E91)-2),""""),IF(MID('[1]HK TREATED'!E91,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E91,LEN('[1]HK TREATED'!E91)-2),""""),IF(H91="-",CONCATENATE("'",'[1]HK TREATED'!E91,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E91,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27395,20 +27395,20 @@
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B92" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C92" s="26"/>
+      <c r="B92" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C92" s="24"/>
       <c r="D92" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F92,4),"""")</f>
         <v>x"0000075A"</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B93" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C93" s="25" t="str">
+      <c r="B93" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C93" s="23" t="str">
         <f>IF('[1]HK TREATED'!E93="-","-",IF(MID('[1]HK TREATED'!E93,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E93,LEN('[1]HK TREATED'!E93)-2),""""),IF(MID('[1]HK TREATED'!E93,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E93,LEN('[1]HK TREATED'!E93)-2),""""),IF(H93="-",CONCATENATE("'",'[1]HK TREATED'!E93,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E93,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27418,20 +27418,20 @@
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B94" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C94" s="26"/>
+      <c r="B94" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C94" s="24"/>
       <c r="D94" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F94,4),"""")</f>
         <v>x"00000758"</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B95" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C95" s="25" t="str">
+      <c r="B95" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C95" s="23" t="str">
         <f>IF('[1]HK TREATED'!E95="-","-",IF(MID('[1]HK TREATED'!E95,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E95,LEN('[1]HK TREATED'!E95)-2),""""),IF(MID('[1]HK TREATED'!E95,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E95,LEN('[1]HK TREATED'!E95)-2),""""),IF(H95="-",CONCATENATE("'",'[1]HK TREATED'!E95,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E95,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27441,20 +27441,20 @@
       </c>
     </row>
     <row r="96" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C96" s="26"/>
+      <c r="B96" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C96" s="24"/>
       <c r="D96" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F96,4),"""")</f>
         <v>x"0000075E"</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B97" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C97" s="25" t="str">
+      <c r="B97" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C97" s="23" t="str">
         <f>IF('[1]HK TREATED'!E97="-","-",IF(MID('[1]HK TREATED'!E97,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E97,LEN('[1]HK TREATED'!E97)-2),""""),IF(MID('[1]HK TREATED'!E97,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E97,LEN('[1]HK TREATED'!E97)-2),""""),IF(H97="-",CONCATENATE("'",'[1]HK TREATED'!E97,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E97,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27464,20 +27464,20 @@
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B98" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C98" s="26"/>
+      <c r="B98" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C98" s="24"/>
       <c r="D98" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F98,4),"""")</f>
         <v>x"0000075C"</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B99" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C99" s="25" t="str">
+      <c r="B99" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C99" s="23" t="str">
         <f>IF('[1]HK TREATED'!E99="-","-",IF(MID('[1]HK TREATED'!E99,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E99,LEN('[1]HK TREATED'!E99)-2),""""),IF(MID('[1]HK TREATED'!E99,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E99,LEN('[1]HK TREATED'!E99)-2),""""),IF(H99="-",CONCATENATE("'",'[1]HK TREATED'!E99,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E99,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27487,20 +27487,20 @@
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B100" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C100" s="26"/>
+      <c r="B100" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C100" s="24"/>
       <c r="D100" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F100,4),"""")</f>
         <v>x"00000762"</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B101" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C101" s="25" t="str">
+      <c r="B101" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C101" s="23" t="str">
         <f>IF('[1]HK TREATED'!E101="-","-",IF(MID('[1]HK TREATED'!E101,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E101,LEN('[1]HK TREATED'!E101)-2),""""),IF(MID('[1]HK TREATED'!E101,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E101,LEN('[1]HK TREATED'!E101)-2),""""),IF(H101="-",CONCATENATE("'",'[1]HK TREATED'!E101,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E101,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27510,20 +27510,20 @@
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B102" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C102" s="26"/>
+      <c r="B102" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C102" s="24"/>
       <c r="D102" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F102,4),"""")</f>
         <v>x"00000760"</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B103" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C103" s="25" t="str">
+      <c r="B103" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C103" s="23" t="str">
         <f>IF('[1]HK TREATED'!E103="-","-",IF(MID('[1]HK TREATED'!E103,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E103,LEN('[1]HK TREATED'!E103)-2),""""),IF(MID('[1]HK TREATED'!E103,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E103,LEN('[1]HK TREATED'!E103)-2),""""),IF(H103="-",CONCATENATE("'",'[1]HK TREATED'!E103,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E103,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27533,20 +27533,20 @@
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B104" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C104" s="26"/>
+      <c r="B104" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C104" s="24"/>
       <c r="D104" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F104,4),"""")</f>
         <v>x"00000766"</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B105" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C105" s="25" t="str">
+      <c r="B105" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C105" s="23" t="str">
         <f>IF('[1]HK TREATED'!E105="-","-",IF(MID('[1]HK TREATED'!E105,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E105,LEN('[1]HK TREATED'!E105)-2),""""),IF(MID('[1]HK TREATED'!E105,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E105,LEN('[1]HK TREATED'!E105)-2),""""),IF(H105="-",CONCATENATE("'",'[1]HK TREATED'!E105,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E105,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27556,20 +27556,20 @@
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B106" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C106" s="26"/>
+      <c r="B106" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C106" s="24"/>
       <c r="D106" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F106,4),"""")</f>
         <v>x"00000764"</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B107" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C107" s="25" t="str">
+      <c r="B107" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C107" s="23" t="str">
         <f>IF('[1]HK TREATED'!E107="-","-",IF(MID('[1]HK TREATED'!E107,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E107,LEN('[1]HK TREATED'!E107)-2),""""),IF(MID('[1]HK TREATED'!E107,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E107,LEN('[1]HK TREATED'!E107)-2),""""),IF(H107="-",CONCATENATE("'",'[1]HK TREATED'!E107,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E107,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27579,20 +27579,20 @@
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B108" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C108" s="26"/>
+      <c r="B108" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C108" s="24"/>
       <c r="D108" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F108,4),"""")</f>
         <v>x"0000076A"</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B109" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C109" s="25" t="str">
+      <c r="B109" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C109" s="23" t="str">
         <f>IF('[1]HK TREATED'!E109="-","-",IF(MID('[1]HK TREATED'!E109,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E109,LEN('[1]HK TREATED'!E109)-2),""""),IF(MID('[1]HK TREATED'!E109,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E109,LEN('[1]HK TREATED'!E109)-2),""""),IF(H109="-",CONCATENATE("'",'[1]HK TREATED'!E109,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E109,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27602,20 +27602,20 @@
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B110" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C110" s="26"/>
+      <c r="B110" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C110" s="24"/>
       <c r="D110" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F110,4),"""")</f>
         <v>x"00000768"</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B111" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C111" s="25" t="str">
+      <c r="B111" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C111" s="23" t="str">
         <f>IF('[1]HK TREATED'!E111="-","-",IF(MID('[1]HK TREATED'!E111,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E111,LEN('[1]HK TREATED'!E111)-2),""""),IF(MID('[1]HK TREATED'!E111,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E111,LEN('[1]HK TREATED'!E111)-2),""""),IF(H111="-",CONCATENATE("'",'[1]HK TREATED'!E111,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E111,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27625,20 +27625,20 @@
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B112" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C112" s="26"/>
+      <c r="B112" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C112" s="24"/>
       <c r="D112" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F112,4),"""")</f>
         <v>x"0000076E"</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B113" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C113" s="25" t="str">
+      <c r="B113" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C113" s="23" t="str">
         <f>IF('[1]HK TREATED'!E113="-","-",IF(MID('[1]HK TREATED'!E113,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E113,LEN('[1]HK TREATED'!E113)-2),""""),IF(MID('[1]HK TREATED'!E113,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E113,LEN('[1]HK TREATED'!E113)-2),""""),IF(H113="-",CONCATENATE("'",'[1]HK TREATED'!E113,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E113,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27648,20 +27648,20 @@
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B114" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C114" s="26"/>
+      <c r="B114" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C114" s="24"/>
       <c r="D114" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F114,4),"""")</f>
         <v>x"0000076C"</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B115" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C115" s="25" t="str">
+      <c r="B115" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C115" s="23" t="str">
         <f>IF('[1]HK TREATED'!E115="-","-",IF(MID('[1]HK TREATED'!E115,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E115,LEN('[1]HK TREATED'!E115)-2),""""),IF(MID('[1]HK TREATED'!E115,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E115,LEN('[1]HK TREATED'!E115)-2),""""),IF(H115="-",CONCATENATE("'",'[1]HK TREATED'!E115,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E115,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27671,20 +27671,20 @@
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B116" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C116" s="26"/>
+      <c r="B116" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C116" s="24"/>
       <c r="D116" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F116,4),"""")</f>
         <v>x"00000772"</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B117" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C117" s="25" t="str">
+      <c r="B117" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C117" s="23" t="str">
         <f>IF('[1]HK TREATED'!E117="-","-",IF(MID('[1]HK TREATED'!E117,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E117,LEN('[1]HK TREATED'!E117)-2),""""),IF(MID('[1]HK TREATED'!E117,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E117,LEN('[1]HK TREATED'!E117)-2),""""),IF(H117="-",CONCATENATE("'",'[1]HK TREATED'!E117,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E117,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27694,20 +27694,20 @@
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B118" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C118" s="26"/>
+      <c r="B118" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C118" s="24"/>
       <c r="D118" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F118,4),"""")</f>
         <v>x"00000770"</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B119" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C119" s="25" t="str">
+      <c r="B119" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C119" s="23" t="str">
         <f>IF('[1]HK TREATED'!E119="-","-",IF(MID('[1]HK TREATED'!E119,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E119,LEN('[1]HK TREATED'!E119)-2),""""),IF(MID('[1]HK TREATED'!E119,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E119,LEN('[1]HK TREATED'!E119)-2),""""),IF(H119="-",CONCATENATE("'",'[1]HK TREATED'!E119,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E119,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27717,20 +27717,20 @@
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B120" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C120" s="26"/>
+      <c r="B120" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C120" s="24"/>
       <c r="D120" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F120,4),"""")</f>
         <v>x"00000776"</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B121" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C121" s="25" t="str">
+      <c r="B121" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C121" s="23" t="str">
         <f>IF('[1]HK TREATED'!E121="-","-",IF(MID('[1]HK TREATED'!E121,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E121,LEN('[1]HK TREATED'!E121)-2),""""),IF(MID('[1]HK TREATED'!E121,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E121,LEN('[1]HK TREATED'!E121)-2),""""),IF(H121="-",CONCATENATE("'",'[1]HK TREATED'!E121,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E121,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27740,20 +27740,20 @@
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B122" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C122" s="26"/>
+      <c r="B122" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C122" s="24"/>
       <c r="D122" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F122,4),"""")</f>
         <v>x"00000774"</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B123" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C123" s="25" t="str">
+      <c r="B123" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C123" s="23" t="str">
         <f>IF('[1]HK TREATED'!E123="-","-",IF(MID('[1]HK TREATED'!E123,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E123,LEN('[1]HK TREATED'!E123)-2),""""),IF(MID('[1]HK TREATED'!E123,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E123,LEN('[1]HK TREATED'!E123)-2),""""),IF(H123="-",CONCATENATE("'",'[1]HK TREATED'!E123,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E123,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27763,20 +27763,20 @@
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B124" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C124" s="26"/>
+      <c r="B124" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C124" s="24"/>
       <c r="D124" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F124,4),"""")</f>
         <v>x"0000077A"</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B125" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C125" s="25" t="str">
+      <c r="B125" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C125" s="23" t="str">
         <f>IF('[1]HK TREATED'!E125="-","-",IF(MID('[1]HK TREATED'!E125,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E125,LEN('[1]HK TREATED'!E125)-2),""""),IF(MID('[1]HK TREATED'!E125,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E125,LEN('[1]HK TREATED'!E125)-2),""""),IF(H125="-",CONCATENATE("'",'[1]HK TREATED'!E125,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E125,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27786,20 +27786,20 @@
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B126" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C126" s="26"/>
+      <c r="B126" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C126" s="24"/>
       <c r="D126" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F126,4),"""")</f>
         <v>x"00000778"</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B127" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C127" s="25" t="str">
+      <c r="B127" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C127" s="23" t="str">
         <f>IF('[1]HK TREATED'!E127="-","-",IF(MID('[1]HK TREATED'!E127,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E127,LEN('[1]HK TREATED'!E127)-2),""""),IF(MID('[1]HK TREATED'!E127,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E127,LEN('[1]HK TREATED'!E127)-2),""""),IF(H127="-",CONCATENATE("'",'[1]HK TREATED'!E127,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E127,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27809,20 +27809,20 @@
       </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B128" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C128" s="26"/>
+      <c r="B128" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C128" s="24"/>
       <c r="D128" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F128,4),"""")</f>
         <v>x"0000077E"</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B129" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C129" s="25" t="str">
+      <c r="B129" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C129" s="23" t="str">
         <f>IF('[1]HK TREATED'!E129="-","-",IF(MID('[1]HK TREATED'!E129,2,1)="x",CONCATENATE("x""",RIGHT('[1]HK TREATED'!E129,LEN('[1]HK TREATED'!E129)-2),""""),IF(MID('[1]HK TREATED'!E129,2,1)="b",CONCATENATE("""",RIGHT('[1]HK TREATED'!E129,LEN('[1]HK TREATED'!E129)-2),""""),IF(H129="-",CONCATENATE("'",'[1]HK TREATED'!E129,"'"),CONCATENATE("(others =&gt; '",'[1]HK TREATED'!E129,"')")))))</f>
         <v>x"FFFF"</v>
       </c>
@@ -27832,10 +27832,10 @@
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B130" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C130" s="26"/>
+      <c r="B130" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C130" s="24"/>
       <c r="D130" s="12" t="str">
         <f>CONCATENATE("x""0000",RIGHT('[1]HK TREATED'!F130,4),"""")</f>
         <v>x"0000077C"</v>
@@ -27843,28 +27843,88 @@
     </row>
   </sheetData>
   <mergeCells count="128">
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B123:B124"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="B127:B128"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="B119:B120"/>
+    <mergeCell ref="B121:B122"/>
+    <mergeCell ref="B105:B106"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="C129:C130"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="C117:C118"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
@@ -27889,88 +27949,28 @@
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="C129:C130"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C105:C106"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C115:C116"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B105:B106"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="B123:B124"/>
-    <mergeCell ref="B125:B126"/>
-    <mergeCell ref="B127:B128"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="B115:B116"/>
-    <mergeCell ref="B117:B118"/>
-    <mergeCell ref="B119:B120"/>
-    <mergeCell ref="B121:B122"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -27995,7 +27995,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>14</v>
@@ -28016,7 +28016,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>13</v>
@@ -28037,7 +28037,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="0"/>
@@ -28049,7 +28049,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>13</v>
@@ -28070,7 +28070,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
@@ -28082,7 +28082,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>13</v>
@@ -28103,7 +28103,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
@@ -28115,7 +28115,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>13</v>
@@ -28136,7 +28136,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
@@ -28148,7 +28148,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>13</v>
@@ -28169,7 +28169,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -28181,7 +28181,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>13</v>
@@ -28202,7 +28202,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
@@ -28214,7 +28214,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>13</v>
@@ -28235,7 +28235,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
@@ -28247,7 +28247,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>13</v>
@@ -28268,7 +28268,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
@@ -28280,7 +28280,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>13</v>
@@ -28301,7 +28301,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
@@ -28313,7 +28313,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>13</v>
@@ -28334,7 +28334,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
@@ -28346,7 +28346,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>13</v>
@@ -28367,7 +28367,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
@@ -28379,7 +28379,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>13</v>
@@ -28400,7 +28400,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
@@ -28412,7 +28412,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>13</v>
@@ -28433,7 +28433,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
@@ -28445,7 +28445,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>13</v>
@@ -28466,7 +28466,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
@@ -28478,7 +28478,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>13</v>
@@ -28499,7 +28499,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
@@ -28511,7 +28511,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>13</v>
@@ -28532,7 +28532,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
@@ -28544,7 +28544,7 @@
         <v>21</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>13</v>
@@ -28565,7 +28565,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
@@ -28577,7 +28577,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>13</v>
@@ -28598,7 +28598,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
@@ -28610,7 +28610,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>13</v>
@@ -28631,7 +28631,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
@@ -28643,7 +28643,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>13</v>
@@ -28664,7 +28664,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="0"/>
@@ -28676,7 +28676,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>13</v>
@@ -28697,7 +28697,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="0"/>
@@ -28709,7 +28709,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>13</v>
@@ -28730,7 +28730,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="0"/>
@@ -28742,7 +28742,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>13</v>
@@ -28763,7 +28763,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="0"/>
@@ -28775,7 +28775,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>13</v>
@@ -28796,7 +28796,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="0"/>
@@ -28808,7 +28808,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>13</v>
@@ -28829,7 +28829,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="0"/>
@@ -28841,7 +28841,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>13</v>
@@ -28862,7 +28862,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="0"/>
@@ -28874,7 +28874,7 @@
         <v>21</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>13</v>
@@ -28895,7 +28895,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="0"/>
@@ -28907,7 +28907,7 @@
         <v>21</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>13</v>
@@ -28928,7 +28928,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="0"/>
@@ -28940,7 +28940,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>13</v>
@@ -28961,7 +28961,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="0"/>
@@ -28973,7 +28973,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>13</v>
@@ -28994,7 +28994,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="0"/>
@@ -29006,7 +29006,7 @@
         <v>21</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>13</v>
@@ -29027,7 +29027,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="0"/>
@@ -29039,7 +29039,7 @@
         <v>21</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>13</v>
@@ -29060,7 +29060,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" ref="L34:L67" si="1">CONCATENATE(B34,C34,D34,E34,F34,G34,H34,I34,J34)</f>
@@ -29072,7 +29072,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>13</v>
@@ -29093,7 +29093,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="1"/>
@@ -29105,7 +29105,7 @@
         <v>21</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>13</v>
@@ -29126,7 +29126,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" si="1"/>
@@ -29138,7 +29138,7 @@
         <v>21</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>13</v>
@@ -29159,7 +29159,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="1"/>
@@ -29171,7 +29171,7 @@
         <v>21</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>13</v>
@@ -29192,7 +29192,7 @@
         <v>0</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" si="1"/>
@@ -29204,7 +29204,7 @@
         <v>21</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>13</v>
@@ -29225,7 +29225,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" si="1"/>
@@ -29237,7 +29237,7 @@
         <v>21</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>13</v>
@@ -29258,7 +29258,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" si="1"/>
@@ -29270,7 +29270,7 @@
         <v>21</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>13</v>
@@ -29291,7 +29291,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" si="1"/>
@@ -29303,7 +29303,7 @@
         <v>21</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>13</v>
@@ -29324,7 +29324,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="1"/>
@@ -29336,7 +29336,7 @@
         <v>21</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>13</v>
@@ -29357,7 +29357,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" si="1"/>
@@ -29369,7 +29369,7 @@
         <v>21</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>13</v>
@@ -29390,7 +29390,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" si="1"/>
@@ -29402,7 +29402,7 @@
         <v>21</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>13</v>
@@ -29423,7 +29423,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" si="1"/>
@@ -29435,7 +29435,7 @@
         <v>21</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>13</v>
@@ -29456,7 +29456,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" si="1"/>
@@ -29468,7 +29468,7 @@
         <v>21</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>13</v>
@@ -29489,7 +29489,7 @@
         <v>0</v>
       </c>
       <c r="J47" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" si="1"/>
@@ -29501,7 +29501,7 @@
         <v>21</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>13</v>
@@ -29522,7 +29522,7 @@
         <v>0</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L48" t="str">
         <f t="shared" si="1"/>
@@ -29534,7 +29534,7 @@
         <v>21</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>13</v>
@@ -29555,7 +29555,7 @@
         <v>0</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" si="1"/>
@@ -29567,7 +29567,7 @@
         <v>21</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>13</v>
@@ -29588,7 +29588,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" si="1"/>
@@ -29600,7 +29600,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>13</v>
@@ -29621,7 +29621,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" si="1"/>
@@ -29633,7 +29633,7 @@
         <v>21</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>13</v>
@@ -29654,7 +29654,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" si="1"/>
@@ -29666,7 +29666,7 @@
         <v>21</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>13</v>
@@ -29687,7 +29687,7 @@
         <v>0</v>
       </c>
       <c r="J53" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L53" t="str">
         <f t="shared" si="1"/>
@@ -29699,7 +29699,7 @@
         <v>21</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>13</v>
@@ -29720,7 +29720,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L54" t="str">
         <f t="shared" si="1"/>
@@ -29732,7 +29732,7 @@
         <v>21</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>13</v>
@@ -29753,7 +29753,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" si="1"/>
@@ -29765,7 +29765,7 @@
         <v>21</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>13</v>
@@ -29786,7 +29786,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" si="1"/>
@@ -29798,7 +29798,7 @@
         <v>21</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>13</v>
@@ -29819,7 +29819,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" si="1"/>
@@ -29831,7 +29831,7 @@
         <v>21</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>13</v>
@@ -29852,7 +29852,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" si="1"/>
@@ -29864,7 +29864,7 @@
         <v>21</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>13</v>
@@ -29885,7 +29885,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L59" t="str">
         <f t="shared" si="1"/>
@@ -29897,7 +29897,7 @@
         <v>21</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>13</v>
@@ -29918,7 +29918,7 @@
         <v>0</v>
       </c>
       <c r="J60" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L60" t="str">
         <f t="shared" si="1"/>
@@ -29930,7 +29930,7 @@
         <v>21</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>13</v>
@@ -29951,7 +29951,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L61" t="str">
         <f t="shared" si="1"/>
@@ -29963,7 +29963,7 @@
         <v>21</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>13</v>
@@ -29984,7 +29984,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" si="1"/>
@@ -29996,7 +29996,7 @@
         <v>21</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>13</v>
@@ -30017,7 +30017,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L63" t="str">
         <f t="shared" si="1"/>
@@ -30029,7 +30029,7 @@
         <v>21</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>13</v>
@@ -30050,7 +30050,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L64" t="str">
         <f t="shared" si="1"/>
@@ -30062,7 +30062,7 @@
         <v>21</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>13</v>
@@ -30083,7 +30083,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" si="1"/>
@@ -30095,7 +30095,7 @@
         <v>21</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>13</v>
@@ -30116,7 +30116,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L66" t="str">
         <f t="shared" si="1"/>
@@ -30154,7 +30154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S268"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10:S265"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -30175,18 +30177,18 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -30204,7 +30206,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S2" t="str">
         <f>CONCATENATE(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2)</f>
@@ -30213,13 +30215,13 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -30246,7 +30248,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S3" t="str">
         <f>CONCATENATE(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3,P3,Q3)</f>
@@ -30255,15 +30257,15 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>38</v>
@@ -30297,7 +30299,7 @@
       </c>
       <c r="S6" t="str">
         <f>CONCATENATE(B6,C6,D6,E6,F6,G6,H6,I6,J6,K6,L6,M6,N6,O6,P6,Q6)</f>
-        <v>signal s_rmap_read_address  : std_logic_vector(31 downto 0);</v>
+        <v>signal rd_addr_i(31 downto 0)  : std_logic_vector(31 downto 0);</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -30311,7 +30313,7 @@
       </c>
       <c r="C9" s="7" t="str">
         <f>C6</f>
-        <v>s_rmap_read_address</v>
+        <v>rd_addr_i(31 downto 0)</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>34</v>
@@ -30331,7 +30333,7 @@
       <c r="Q9" s="5"/>
       <c r="S9" t="str">
         <f t="shared" ref="S9:S72" si="0">CONCATENATE(B9,C9,D9,E9,F9,G9,H9,I9,J9,K9,L9,M9,N9,O9,P9,Q9)</f>
-        <v>case (s_rmap_read_address) is</v>
+        <v>case (rd_addr_i(31 downto 0)) is</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -41194,7 +41196,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:X332"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A283" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X269" sqref="X269:X332"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -41224,18 +41228,18 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -41269,7 +41273,7 @@
         <v>17</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X2" t="str">
         <f>CONCATENATE(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2)</f>
@@ -41278,13 +41282,13 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -41307,7 +41311,7 @@
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X3" t="str">
         <f>CONCATENATE(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3,P3,Q3,R3,S3,T3,U3,V3)</f>
@@ -41316,15 +41320,15 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>38</v>
@@ -41365,7 +41369,7 @@
       </c>
       <c r="X6" t="str">
         <f>CONCATENATE(B6,C6,D6,E6,F6,G6,H6,I6,J6,K6,L6,M6,N6,O6,P6,Q6,R6,S6,T6,U6,V6)</f>
-        <v>signal s_rmap_write_address  : std_logic_vector(31 downto 0);</v>
+        <v>signal wr_addr_i(31 downto 0)  : std_logic_vector(31 downto 0);</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
@@ -41379,13 +41383,13 @@
       </c>
       <c r="C9" s="7" t="str">
         <f>$C$6</f>
-        <v>s_rmap_write_address</v>
+        <v>wr_addr_i(31 downto 0)</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -41406,7 +41410,7 @@
       <c r="V9" s="5"/>
       <c r="X9" t="str">
         <f t="shared" ref="X9:X72" si="0">CONCATENATE(B9,C9,D9,E9,F9,G9,H9,I9,J9,K9,L9,M9,N9,O9,P9,Q9,R9,S9,T9,U9,V9)</f>
-        <v>case (s_rmap_write_address) is</v>
+        <v>case (wr_addr_i(31 downto 0)) is</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -53472,7 +53476,7 @@
     </row>
     <row r="268" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A268" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="269" spans="1:24" x14ac:dyDescent="0.3">

</xml_diff>